<commit_message>
fix sql script, change list cert to table
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhucTri\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD8AEFE-86D7-400D-A54A-0BA98CEC77FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746E3245-D9F4-4751-AA66-C5234FAA4647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -111,6 +111,9 @@
     <t>Sáo</t>
   </si>
   <si>
+    <t>ĐTR101</t>
+  </si>
+  <si>
     <t>ĐH200304</t>
   </si>
   <si>
@@ -120,19 +123,10 @@
     <t>Phạm Thanh Hà</t>
   </si>
   <si>
-    <t xml:space="preserve">Vovinam 1 </t>
-  </si>
-  <si>
-    <t>Vovinam 2</t>
-  </si>
-  <si>
-    <t>VOV101</t>
-  </si>
-  <si>
-    <t>VOV102</t>
-  </si>
-  <si>
-    <t>SAO100</t>
+    <t>Lừa trái tim đàn bà</t>
+  </si>
+  <si>
+    <t>Tình một đêm</t>
   </si>
 </sst>
 </file>
@@ -452,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,10 +507,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -551,10 +545,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -572,13 +566,13 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="J3">
         <v>7.5</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -589,10 +583,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -610,13 +604,13 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -627,10 +621,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -648,16 +642,16 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix validate import excel, create campus
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>No</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Hoàng Việt Bách</t>
+  </si>
+  <si>
+    <t>Hoàng      Việt Bách</t>
   </si>
 </sst>
 </file>
@@ -446,25 +449,25 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="36.28515625" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="36.33203125" customWidth="1"/>
+    <col min="12" max="12" width="33.44140625" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -510,7 +513,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -540,7 +543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -578,7 +581,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -616,7 +619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Add account web service
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ha\OneDrive\Desktop\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\New folder (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248DDAE2-35D9-4AB6-95E2-324862AA4C4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFB1166-6BB7-4269-A24D-7CCCBA84EB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-96" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>ÐTR101</t>
   </si>
   <si>
-    <t>Đàn tranh</t>
-  </si>
-  <si>
     <t>Nam</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>ĐH200305</t>
+  </si>
+  <si>
+    <t>Đàn tranh 123</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,10 +508,10 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
         <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -519,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
         <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -546,10 +546,10 @@
         <v>8.1</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -557,19 +557,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -584,10 +584,10 @@
         <v>7.5</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -595,19 +595,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -622,10 +622,10 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -633,13 +633,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -654,16 +654,16 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5">
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -671,16 +671,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -692,16 +692,16 @@
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6">
         <v>10</v>
       </c>
       <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
         <v>36</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug get list of campus
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BachHV\Desktop\New folder (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFB1166-6BB7-4269-A24D-7CCCBA84EB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -75,6 +74,9 @@
     <t>ÐTR101</t>
   </si>
   <si>
+    <t>Đàn tranh</t>
+  </si>
+  <si>
     <t>Nam</t>
   </si>
   <si>
@@ -114,37 +116,28 @@
     <t>ĐH200304</t>
   </si>
   <si>
-    <t>HE130576</t>
-  </si>
-  <si>
-    <t>Phạm Thanh Hà</t>
-  </si>
-  <si>
-    <t>Lừa trái tim đàn bà</t>
-  </si>
-  <si>
-    <t>Tình một đêm</t>
-  </si>
-  <si>
-    <t>26/09/1999</t>
-  </si>
-  <si>
-    <t>ABC101</t>
-  </si>
-  <si>
-    <t>Học</t>
+    <t>HE130585</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc Hải</t>
+  </si>
+  <si>
+    <t>Vovinam 1</t>
+  </si>
+  <si>
+    <t>Vovinam 2</t>
+  </si>
+  <si>
+    <t>Vovinam 3</t>
   </si>
   <si>
     <t>ĐH200305</t>
-  </si>
-  <si>
-    <t>Đàn tranh 123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,11 +448,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +467,7 @@
     <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="36.28515625" customWidth="1"/>
     <col min="12" max="12" width="33.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -508,10 +502,10 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -519,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -546,10 +540,10 @@
         <v>8.1</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -557,19 +551,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -587,7 +581,7 @@
         <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -595,19 +589,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -622,10 +616,10 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -633,13 +627,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -654,16 +648,16 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -671,16 +665,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -692,16 +686,16 @@
         <v>14</v>
       </c>
       <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6" t="s">
         <v>34</v>
       </c>
-      <c r="J6">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>35</v>
-      </c>
-      <c r="L6" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix load all edu system
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>No</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>ĐH200305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Nguyễn Ngọc    Hải</t>
+  </si>
+  <si>
+    <t>Nguyễn    Ngọc Hải</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc              Hải</t>
   </si>
 </sst>
 </file>
@@ -452,7 +461,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D14" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +525,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -592,7 +601,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -668,7 +677,7 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
test super admin role 23/04
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\New folder (2)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFB1166-6BB7-4269-A24D-7CCCBA84EB9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F814182-812F-4F2A-A66F-6933D22278B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>No</t>
   </si>
@@ -139,16 +139,25 @@
   </si>
   <si>
     <t>Đàn tranh 123</t>
+  </si>
+  <si>
+    <t>HE130577</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,7 +468,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -705,6 +714,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix function unit test
</commit_message>
<xml_diff>
--- a/eCert/Uploads/Nhac-cu-dan-toc.xlsx
+++ b/eCert/Uploads/Nhac-cu-dan-toc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>No</t>
   </si>
@@ -131,10 +131,13 @@
     <t>ĐH200305</t>
   </si>
   <si>
-    <t>HE130 585</t>
-  </si>
-  <si>
     <t>ĐH2003 04</t>
+  </si>
+  <si>
+    <t>Phạm Thanh Hà</t>
+  </si>
+  <si>
+    <t>HE130576</t>
   </si>
 </sst>
 </file>
@@ -455,7 +458,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,10 +519,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -630,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -660,7 +663,7 @@
         <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>